<commit_message>
contain duplicate II , array
</commit_message>
<xml_diff>
--- a/qns_track/DSA-qns doubt sheet.xlsx
+++ b/qns_track/DSA-qns doubt sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA c++\qns_track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F657A4-60A6-49E0-84B2-E565DAEC70FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9930D46B-07BA-486E-8914-DC3284DC3245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E25C5EDD-CE4D-41E6-B072-45BA83DAA013}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Solved or Not</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>Single number (unique no. in array)</t>
+  </si>
+  <si>
+    <t>Majority element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/description/</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Moore's voting algo.</t>
   </si>
 </sst>
 </file>
@@ -459,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE397DD1-9FD4-46F8-AAB9-6343BD54286E}">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +492,7 @@
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -502,8 +517,11 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -529,7 +547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -555,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -581,7 +599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -589,7 +607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -613,6 +631,35 @@
       </c>
       <c r="K7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -621,8 +668,9 @@
     <hyperlink ref="C4" r:id="rId2" xr:uid="{E9327DA6-6904-41A5-B16D-1F1B5B77ECF9}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{4933DB51-C4FA-4D2F-BCD2-D9BC67C85E64}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{B04DE82C-6F3B-44EF-BE91-7B5CE95BD706}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{6801DCE9-CA55-4ED1-BEDA-04F04B2CE498}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>